<commit_message>
added some mapping functions
</commit_message>
<xml_diff>
--- a/data-raw/eex_ddh_JSON_lookup_basic.xlsx
+++ b/data-raw/eex_ddh_JSON_lookup_basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FA2B98-9252-439F-B381-89059F84A44E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F37744-3880-49A4-8BB2-301F3B250A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>eex_field_JSON</t>
   </si>
@@ -34,54 +34,48 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>$id</t>
-  </si>
-  <si>
-    <t>$title</t>
-  </si>
-  <si>
-    <t>$notes</t>
-  </si>
-  <si>
-    <t>$release_date</t>
-  </si>
-  <si>
-    <t>$end_date</t>
-  </si>
-  <si>
-    <t>$author_email</t>
-  </si>
-  <si>
-    <t>$start_date</t>
-  </si>
-  <si>
-    <t>$author</t>
-  </si>
-  <si>
-    <t>$url</t>
-  </si>
-  <si>
-    <t>$metadata_modified</t>
-  </si>
-  <si>
-    <t>$description</t>
-  </si>
-  <si>
-    <t>$name</t>
-  </si>
-  <si>
-    <t>$country_code</t>
-  </si>
-  <si>
-    <t>$region</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>author_email</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>metadata_modified</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>region</t>
   </si>
   <si>
     <t>field_ddh_harvest_sys_id</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>body</t>
   </si>
   <si>
@@ -121,11 +115,14 @@
     <t>FALSE</t>
   </si>
   <si>
-    <t>Tim used $content$result$metadata_created,_x000D__x000D__x000D_
+    <t>Tim used $content$result$metadata_created,_x000D__x000D__x000D__x000D_
 Need to account for converting if only years give e.g 2010 to 01/01/2010</t>
   </si>
   <si>
     <t>Need to account for converting if only years give e.g 2010 to 01/01/2010</t>
+  </si>
+  <si>
+    <t>metadata_created</t>
   </si>
 </sst>
 </file>
@@ -480,11 +477,13 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="108.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,10 +506,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,10 +517,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,154 +528,155 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix resource url mapping for geojson and update dataset_json_lookup
</commit_message>
<xml_diff>
--- a/data-raw/eex_ddh_JSON_lookup_basic.xlsx
+++ b/data-raw/eex_ddh_JSON_lookup_basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEA49B0-0C8E-4DBF-87EA-BAC857AA944E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE84F517-1084-4E8C-B406-979A2C170A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>eex_field_JSON</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>license_title</t>
-  </si>
-  <si>
-    <t>field_link_api</t>
   </si>
 </sst>
 </file>
@@ -480,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,21 +647,21 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -672,34 +669,23 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reverted changes, changes are present in fix_geoJSON local branch
</commit_message>
<xml_diff>
--- a/data-raw/eex_ddh_JSON_lookup_basic.xlsx
+++ b/data-raw/eex_ddh_JSON_lookup_basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB525812\cmder\Git Repos\eex2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE84F517-1084-4E8C-B406-979A2C170A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337015D8-0216-4F04-A4E3-B0AAECF60A42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>eex_field_JSON</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>license_title</t>
+  </si>
+  <si>
+    <t>field_link_api</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,6 +692,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>